<commit_message>
Alter table idea, ERD, fix bugs, add methods, etc.
</commit_message>
<xml_diff>
--- a/Idea of Tables.xlsx
+++ b/Idea of Tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufr\OneDrive\Desktop\Lessons\Database\Assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufr\OneDrive\Documents\GitHub\dbs-as2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86CD3DE-29C5-4BE1-9E9F-12B7263724F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935D0D1C-F1B2-47EB-AA66-3BE09B6B0C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{222325C7-C5FF-49BE-A5A5-C40156CF4F3F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -95,19 +95,22 @@
     <t>CustomerID (PK)</t>
   </si>
   <si>
-    <t>TotalPrice</t>
-  </si>
-  <si>
     <t>BookOrderInfo</t>
   </si>
   <si>
-    <t>OrderID (FK)</t>
-  </si>
-  <si>
     <t>BookID (PK)</t>
   </si>
   <si>
-    <t>BookID (FK)</t>
+    <t>OrderID (PK, FK)</t>
+  </si>
+  <si>
+    <t>BookID (PK, FK)</t>
+  </si>
+  <si>
+    <t>BookAuthorInfo</t>
+  </si>
+  <si>
+    <t>AuthorID (PK, FK)</t>
   </si>
 </sst>
 </file>
@@ -231,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -256,6 +259,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7167D98D-3AC3-4B22-BB9E-74BAE5ADA01E}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,8 +592,8 @@
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
@@ -617,7 +625,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -788,7 +796,7 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="D18" s="12"/>
       <c r="G18" s="8" t="s">
         <v>13</v>
       </c>
@@ -803,7 +811,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="D19" s="12"/>
       <c r="G19" s="10"/>
       <c r="H19" s="11"/>
       <c r="J19" s="7"/>
@@ -813,15 +821,13 @@
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="D20" s="13"/>
       <c r="G20" s="3" t="s">
         <v>12</v>
       </c>
@@ -837,9 +843,9 @@
     </row>
     <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="14"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="J21" s="1"/>
@@ -847,9 +853,9 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="14"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="J22" s="1"/>
@@ -857,9 +863,9 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="14"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="J23" s="1"/>
@@ -867,9 +873,9 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="14"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="J24" s="1"/>
@@ -877,9 +883,9 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="14"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="J25" s="1"/>
@@ -887,9 +893,9 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="14"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="J26" s="1"/>
@@ -897,9 +903,9 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="14"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="J27" s="1"/>
@@ -907,9 +913,9 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="14"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="J28" s="1"/>
@@ -917,9 +923,9 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="14"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="J29" s="1"/>
@@ -927,9 +933,9 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="14"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="J30" s="1"/>
@@ -937,9 +943,9 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="14"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="J31" s="1"/>
@@ -947,9 +953,9 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="14"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="J32" s="1"/>
@@ -957,79 +963,114 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="14"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="7"/>
+    </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
+      <c r="G37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B36:C37"/>
     <mergeCell ref="J18:K19"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="G18:H19"/>
-    <mergeCell ref="A18:D19"/>
+    <mergeCell ref="G35:H36"/>
+    <mergeCell ref="A18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Only transaction is left
</commit_message>
<xml_diff>
--- a/Idea of Tables.xlsx
+++ b/Idea of Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufr\OneDrive\Documents\GitHub\dbs-as2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935D0D1C-F1B2-47EB-AA66-3BE09B6B0C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E4901C-2448-492F-9441-44C66041C87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{222325C7-C5FF-49BE-A5A5-C40156CF4F3F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>AuthorName</t>
-  </si>
-  <si>
-    <t>AuthorID (FK)</t>
   </si>
   <si>
     <t>AuthorID (PK)</t>
@@ -150,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -230,11 +227,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -243,6 +258,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,11 +277,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7167D98D-3AC3-4B22-BB9E-74BAE5ADA01E}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,56 +621,53 @@
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -658,10 +677,9 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -669,10 +687,9 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -680,10 +697,9 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -691,10 +707,9 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -702,10 +717,9 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -713,10 +727,9 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -724,10 +737,9 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -735,10 +747,9 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -746,10 +757,9 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -757,10 +767,9 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -768,10 +777,9 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -779,10 +787,9 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="6"/>
@@ -791,51 +798,51 @@
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="12"/>
-      <c r="G18" s="8" t="s">
+      <c r="A18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="7"/>
+      <c r="G18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="7"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="12"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="7"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="5"/>
       <c r="G20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>6</v>
@@ -845,7 +852,6 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="14"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="J21" s="1"/>
@@ -855,7 +861,6 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="14"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="J22" s="1"/>
@@ -865,7 +870,6 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="14"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="J23" s="1"/>
@@ -875,7 +879,6 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="14"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="J24" s="1"/>
@@ -885,7 +888,6 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="14"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="J25" s="1"/>
@@ -895,7 +897,6 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="14"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="J26" s="1"/>
@@ -905,7 +906,6 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="14"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="J27" s="1"/>
@@ -915,7 +915,6 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="14"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="J28" s="1"/>
@@ -925,7 +924,6 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="14"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="J29" s="1"/>
@@ -935,7 +933,6 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="14"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="J30" s="1"/>
@@ -945,7 +942,6 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="14"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="J31" s="1"/>
@@ -955,7 +951,6 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="14"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="J32" s="1"/>
@@ -965,42 +960,41 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="14"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="G37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="G37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -1067,10 +1061,10 @@
   <mergeCells count="6">
     <mergeCell ref="B36:C37"/>
     <mergeCell ref="J18:K19"/>
-    <mergeCell ref="A1:I2"/>
     <mergeCell ref="G18:H19"/>
     <mergeCell ref="G35:H36"/>
     <mergeCell ref="A18:C19"/>
+    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Alter table idea and code based on idea
</commit_message>
<xml_diff>
--- a/Idea of Tables.xlsx
+++ b/Idea of Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raufr\OneDrive\Documents\GitHub\dbs-as2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E4901C-2448-492F-9441-44C66041C87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F81277-9A06-41D9-B4D4-C455AB376AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{222325C7-C5FF-49BE-A5A5-C40156CF4F3F}"/>
   </bookViews>
@@ -249,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -283,6 +283,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -600,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7167D98D-3AC3-4B22-BB9E-74BAE5ADA01E}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +634,7 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-      <c r="I1" s="15"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -643,7 +645,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -802,7 +804,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="7"/>
       <c r="G18" s="9" t="s">
         <v>12</v>
@@ -817,7 +819,7 @@
     <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="7"/>
       <c r="G19" s="11"/>
       <c r="H19" s="12"/>
@@ -831,9 +833,7 @@
       <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="C20" s="16"/>
       <c r="D20" s="5"/>
       <c r="G20" s="3" t="s">
         <v>11</v>
@@ -851,7 +851,7 @@
     <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="15"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="J21" s="1"/>
@@ -860,7 +860,7 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="15"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="J22" s="1"/>
@@ -869,7 +869,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="15"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="J23" s="1"/>
@@ -878,7 +878,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="15"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="J24" s="1"/>
@@ -887,7 +887,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="15"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="J25" s="1"/>
@@ -896,7 +896,7 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="15"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="J26" s="1"/>
@@ -905,7 +905,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="15"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="J27" s="1"/>
@@ -914,7 +914,7 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="15"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="J28" s="1"/>
@@ -923,7 +923,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="15"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="J29" s="1"/>
@@ -932,7 +932,7 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="15"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="J30" s="1"/>
@@ -941,7 +941,7 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="C31" s="15"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="J31" s="1"/>
@@ -950,7 +950,7 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="C32" s="15"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="J32" s="1"/>
@@ -959,7 +959,7 @@
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="C33" s="15"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="J33" s="1"/>
@@ -971,17 +971,19 @@
       </c>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
       <c r="G37" s="3" t="s">
         <v>21</v>
       </c>
@@ -996,75 +998,97 @@
       <c r="C38" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="D38" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="15"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="15"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="B36:D37"/>
+    <mergeCell ref="A18:B19"/>
     <mergeCell ref="J18:K19"/>
     <mergeCell ref="G18:H19"/>
     <mergeCell ref="G35:H36"/>
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>